<commit_message>
update .bat and printing query dataframe
</commit_message>
<xml_diff>
--- a/main_dataframe_database.xlsx
+++ b/main_dataframe_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ16"/>
+  <dimension ref="A1:AJ23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2821,6 +2821,1036 @@
         <v>15</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PB1-2307000305</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>F230316011EH</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1N4148WG-Cu-L10</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>2315</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2023/04/09</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3DS1N4148W0SB01</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>1N4148WG</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>F230316011EH</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>2315</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>2023/04/09</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>3000</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>T4</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>SOD123</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0051</v>
+      </c>
+      <c r="T17" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U17" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V17" t="n">
+        <v>1</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>[3000, 3000, 60000]</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>[3000, 3000, 240000]</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA17" t="n">
+        <v>11</v>
+      </c>
+      <c r="AB17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="AD17" t="n">
+        <v>6277</v>
+      </c>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="n">
+        <v>125</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>3000</v>
+      </c>
+      <c r="AH17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>PB1-2307000305</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>F23031601109</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1N4148WG-Cu-L10</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>2315</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2023/04/09</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>77000</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3DS1N4148W0SB01</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>1N4148WG</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>F23031601109</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>2315</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>2023/04/09</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>77000</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>T4</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>SOD123</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>0.0051</v>
+      </c>
+      <c r="T18" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U18" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V18" t="n">
+        <v>25</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>[17000, 77000, 60000]</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>[1, 1, 1]</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>[77000, 77000, 240000]</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA18" t="n">
+        <v>11</v>
+      </c>
+      <c r="AB18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="AD18" t="n">
+        <v>6281</v>
+      </c>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="n">
+        <v>500</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>3000</v>
+      </c>
+      <c r="AH18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>PB1-2307000305</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>ZR374H600Z0710</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>M4G-100</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2137</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2021/09/05</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3DSGS1G4000SB01</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>M4G</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>ZR374H600Z0710</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>2137</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>2021/09/05</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>15000</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>LSYM M4</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>0.007900000000000001</v>
+      </c>
+      <c r="T19" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U19" t="n">
+        <v>7500</v>
+      </c>
+      <c r="V19" t="n">
+        <v>2</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>[0, 15000, 15000]</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>[0, 1, 1]</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>[15000, 15000, 120000]</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA19" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>X1</t>
+        </is>
+      </c>
+      <c r="AD19" t="n">
+        <v>3090</v>
+      </c>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="n">
+        <v>315</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>7500</v>
+      </c>
+      <c r="AH19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>PB1-2307000305</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>F210813041AC</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>MBRD5100G-L10</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>2148</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2021/11/21</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3DYMBRD5100SB01</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>MBRD5100</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>F210813041AC</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>2148</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>2021/11/21</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>LSYM
+MBRD5100</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>TO252</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>0.1067</v>
+      </c>
+      <c r="T20" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U20" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V20" t="n">
+        <v>2</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>[5000, 5000, 50000]</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>[5000, 5000, 200000]</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA20" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+      <c r="AD20" t="n">
+        <v>3646</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>windows user:
+力神料號
+MBRD10100CTG-LS02</t>
+        </is>
+      </c>
+      <c r="AF20" t="n">
+        <v>200</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AH20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>PB1-2111000268</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>F220322022DK</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>MMSZ5243BG-L10</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>2239</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2022/09/25</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>3DZ013W505S0B02</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>MMSZ5243BG</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>F220322022DK</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>2239</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>2022/09/25</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>H3</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>SOD123</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="T21" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U21" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V21" t="n">
+        <v>2</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>[6000, 6000, 60000]</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>[6000, 6000, 240000]</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA21" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="AD21" t="n">
+        <v>5363</v>
+      </c>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="n">
+        <v>200</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>3000</v>
+      </c>
+      <c r="AH21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>PB1-2308000138</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>H202306201101002</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>P2SD75AG-730</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2325</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2023/06/18</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>3DT075200U0SB01</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>P2SD75AG</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>H202306201101002</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>2325</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>2023/06/18</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>XR</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>SOD123FL</t>
+        </is>
+      </c>
+      <c r="S22" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="T22" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U22" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V22" t="n">
+        <v>2</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>[5000, 5000, 60000]</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>[5000, 5000, 240000]</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA22" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>I2</t>
+        </is>
+      </c>
+      <c r="AD22" t="n">
+        <v>6230</v>
+      </c>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="n">
+        <v>200</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AH22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023/08/15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>I230815001</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>PB1-2105000582</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>協禧微機電</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>F210416513K3</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>P4SMAJ64AG-L10</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2150</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2021/09/26</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>3600</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>3DT064400U0SB03</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>P4SMAJ64AG</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>F210416513K3</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>2150</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2021/09/26</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>3600</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>LSYM
+RM</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="S23" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="T23" t="n">
+        <v>31.64</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1800</v>
+      </c>
+      <c r="V23" t="n">
+        <v>2</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>[3600, 3600, 25200]</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>[3600, 3600, 100800]</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA23" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>A7</t>
+        </is>
+      </c>
+      <c r="AD23" t="n">
+        <v>6086</v>
+      </c>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="n">
+        <v>200</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>1800</v>
+      </c>
+      <c r="AH23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>